<commit_message>
Préparation de la publication 4.0.2 (#210)
* préparation publication 4.0.2

* JDV264

* mode PEC

* JDV

* maj aliases.fsh

* Update aliases.fsh

* Update contenu_dossier.md

* pour publication 2c4d22f92e153160d0507de00f6888fd4b359b3d
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.2-ballot-3</t>
+    <t>4.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-18T17:21:18+00:00</t>
+    <t>2024-07-02T09:49:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
publi 403-ballot (#299) 548630c456e89fe6aeadd8d1d6c3637dc3d39519
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.2</t>
+    <t>4.0.3-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-19T12:46:51+00:00</t>
+    <t>2024-12-19T14:23:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Pour publication release 4.0.4 (#336)
* Pour publication release 4.0.4

* Update release-notes.md

* Update release-notes.md ee84e8dde69f8798b6b2fcec41472926ea1dad3a
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.3</t>
+    <t>4.0.4</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-16T08:35:57+00:00</t>
+    <t>2025-06-18T13:08:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Flux 4  préciser la signification métier de la date de statut (#340)
* modif date statut unité

* Update sushi-config.yaml

* update workflows

* Update SDOTaskInputCS.fsh

* Update SDOTask.fsh

* Update SDOTask.fsh

* Update SDOTask.fsh

* Update SDOTaskInputCS.fsh

---------

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com> 6fe4d2f61f01940b01f087b7afb0d24be1949320
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-19T08:03:00+00:00</t>
+    <t>2025-10-09T08:51:23+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -165,7 +165,7 @@
     <t>dateStatutESMS</t>
   </si>
   <si>
-    <t>Permet de définir la date d'entrée dans le statut</t>
+    <t>La spécification fonctionnelle des échanges (https://esante.gouv.fr/volet-si-esms-viatrajectoire-module-ph) donne la signification de cette date par rapport au statut ESMS</t>
   </si>
   <si>
     <t>idUnite</t>
@@ -213,7 +213,7 @@
     <t>dateStatutUnite</t>
   </si>
   <si>
-    <t>Permet de définir la date d'entrée renseignée par l'utilisateur pour les statuts</t>
+    <t>La spécification fonctionnelle des échanges (https://esante.gouv.fr/volet-si-esms-viatrajectoire-module-ph) donne la signification de cette date par rapport au statut de l’unité</t>
   </si>
   <si>
     <t>motifUnite</t>

</xml_diff>

<commit_message>
Préparation de la release 405 (#342)
* preparation release 405

* ajout Changes

* Update sushi-config.yaml

* Delete release-notes.md 4ec2df190f9ca061fa362b5055824dca0cd1da11
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/main/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.4</t>
+    <t>4.0.5</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-09T08:51:23+00:00</t>
+    <t>2025-10-13T12:40:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>